<commit_message>
Final Version Completed after adding 6 new species & 3 nest records. 1. Added new species and nest records. 2. Adjusted the statistics and pie charts accordingly. 3. Corrected some grammatical errors. 4. Updated the README.md file. 5. Updated the two excel files with the new data. 6. Added the pieCharts.docx file with the pie charts. 7. Compressed the images used in the document for lower file size.
</commit_message>
<xml_diff>
--- a/old_vs_new_records.xlsx
+++ b/old_vs_new_records.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Projects\Mora-Bird-Diversity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D6D563-1EE9-4496-BC91-0D1551B0CDB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF2298ED-2172-48CA-AA52-237460D1D118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1758,7 +1758,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1784,8 +1784,14 @@
       <color theme="1"/>
       <name val="Marker Felt"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1826,12 +1832,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF1C232"/>
         <bgColor rgb="FFF1C232"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1918,7 +1918,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2136,8 +2136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A497" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="A416" workbookViewId="0">
+      <selection activeCell="H439" sqref="H439"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2489,10 +2489,10 @@
       <c r="B34" s="2">
         <v>1</v>
       </c>
-      <c r="C34" s="3"/>
-      <c r="D34" s="16">
-        <v>1</v>
-      </c>
+      <c r="C34" s="3">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1"/>
       <c r="E34" s="1"/>
     </row>
     <row r="35" spans="1:5" ht="15.75" customHeight="1">
@@ -2642,10 +2642,10 @@
       <c r="B47" s="2">
         <v>1</v>
       </c>
-      <c r="C47" s="3"/>
-      <c r="D47" s="7">
-        <v>1</v>
-      </c>
+      <c r="C47" s="3">
+        <v>1</v>
+      </c>
+      <c r="D47" s="1"/>
       <c r="E47" s="1"/>
     </row>
     <row r="48" spans="1:5" ht="15.75" customHeight="1">
@@ -3474,7 +3474,7 @@
       <c r="B135" s="2">
         <v>1</v>
       </c>
-      <c r="C135" s="9">
+      <c r="C135" s="16">
         <v>1</v>
       </c>
       <c r="D135" s="1"/>
@@ -3485,9 +3485,13 @@
         <v>137</v>
       </c>
       <c r="B136" s="2"/>
-      <c r="C136" s="3"/>
+      <c r="C136" s="3">
+        <v>1</v>
+      </c>
       <c r="D136" s="1"/>
-      <c r="E136" s="1"/>
+      <c r="E136" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="137" spans="1:5" ht="15.75" customHeight="1">
       <c r="A137" s="1" t="s">
@@ -3507,9 +3511,13 @@
         <v>139</v>
       </c>
       <c r="B138" s="2"/>
-      <c r="C138" s="3"/>
+      <c r="C138" s="3">
+        <v>1</v>
+      </c>
       <c r="D138" s="1"/>
-      <c r="E138" s="1"/>
+      <c r="E138" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="139" spans="1:5" ht="15.75" customHeight="1">
       <c r="A139" s="1" t="s">
@@ -4621,9 +4629,13 @@
         <v>257</v>
       </c>
       <c r="B256" s="2"/>
-      <c r="C256" s="3"/>
+      <c r="C256" s="3">
+        <v>1</v>
+      </c>
       <c r="D256" s="1"/>
-      <c r="E256" s="1"/>
+      <c r="E256" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="257" spans="1:5" ht="15.75" customHeight="1">
       <c r="A257" s="1" t="s">
@@ -5570,10 +5582,10 @@
       <c r="B351" s="2">
         <v>1</v>
       </c>
-      <c r="C351" s="3"/>
-      <c r="D351" s="7">
-        <v>1</v>
-      </c>
+      <c r="C351" s="3">
+        <v>1</v>
+      </c>
+      <c r="D351" s="1"/>
       <c r="E351" s="1"/>
     </row>
     <row r="352" spans="1:5" ht="15.75" customHeight="1">
@@ -6430,10 +6442,10 @@
       <c r="B439" s="2">
         <v>1</v>
       </c>
-      <c r="C439" s="3"/>
-      <c r="D439" s="7">
-        <v>1</v>
-      </c>
+      <c r="C439" s="3">
+        <v>1</v>
+      </c>
+      <c r="D439" s="1"/>
       <c r="E439" s="1"/>
     </row>
     <row r="440" spans="1:5" ht="15.75" customHeight="1">
@@ -7049,15 +7061,15 @@
       </c>
       <c r="C501" s="3">
         <f t="shared" si="0"/>
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="D501" s="1">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E501" s="1">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="502" spans="1:5" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
Updates with Black Bittern Record. fixes #19
</commit_message>
<xml_diff>
--- a/old_vs_new_records.xlsx
+++ b/old_vs_new_records.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Projects\Mora-Bird-Diversity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF2298ED-2172-48CA-AA52-237460D1D118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65CC9AB1-5F91-4715-AEAB-6CB2DD9849D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1895,7 +1895,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1908,6 +1908,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1918,7 +1919,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2136,24 +2137,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A416" workbookViewId="0">
-      <selection activeCell="H439" sqref="H439"/>
+    <sheetView tabSelected="1" topLeftCell="A488" workbookViewId="0">
+      <selection activeCell="H506" sqref="H506"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="53.42578125" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" customWidth="1"/>
+    <col min="1" max="1" width="53.44140625" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" customWidth="1"/>
     <col min="3" max="3" width="8" customWidth="1"/>
     <col min="4" max="4" width="4" customWidth="1"/>
-    <col min="5" max="5" width="3.85546875" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" customWidth="1"/>
-    <col min="7" max="7" width="3.85546875" customWidth="1"/>
-    <col min="8" max="8" width="30.85546875" customWidth="1"/>
-    <col min="9" max="26" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="3.88671875" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" customWidth="1"/>
+    <col min="7" max="7" width="3.88671875" customWidth="1"/>
+    <col min="8" max="8" width="30.88671875" customWidth="1"/>
+    <col min="9" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" ht="14.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2166,14 +2167,14 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" ht="14.4">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" ht="14.4">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -2185,7 +2186,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" ht="14.4">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -2197,7 +2198,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" ht="14.4">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -2206,7 +2207,7 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" ht="14.4">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -2215,7 +2216,7 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" ht="14.4">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -2224,7 +2225,7 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" ht="14.4">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -2233,7 +2234,7 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" ht="14.4">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -2242,7 +2243,7 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" ht="14.4">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -2251,7 +2252,7 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" ht="14.4">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -2260,7 +2261,7 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" ht="14.4">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -2269,7 +2270,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" ht="14.4">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -2278,7 +2279,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" ht="14.4">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -2287,7 +2288,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" ht="14.4">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -2296,7 +2297,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" ht="14.4">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -2305,7 +2306,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" ht="14.4">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -2314,7 +2315,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" ht="14.4">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -2323,7 +2324,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" ht="14.4">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -2332,7 +2333,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" ht="14.4">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -2620,10 +2621,10 @@
       <c r="B45" s="2">
         <v>1</v>
       </c>
-      <c r="C45" s="3"/>
-      <c r="D45" s="7">
-        <v>1</v>
-      </c>
+      <c r="C45" s="3">
+        <v>1</v>
+      </c>
+      <c r="D45" s="17"/>
       <c r="E45" s="1"/>
     </row>
     <row r="46" spans="1:5" ht="15.75" customHeight="1">
@@ -3474,7 +3475,7 @@
       <c r="B135" s="2">
         <v>1</v>
       </c>
-      <c r="C135" s="16">
+      <c r="C135" s="12">
         <v>1</v>
       </c>
       <c r="D135" s="1"/>
@@ -5477,11 +5478,11 @@
       <c r="A341" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="B341" s="12">
-        <v>1</v>
-      </c>
-      <c r="C341" s="14"/>
-      <c r="D341" s="15">
+      <c r="B341" s="13">
+        <v>1</v>
+      </c>
+      <c r="C341" s="15"/>
+      <c r="D341" s="16">
         <v>1</v>
       </c>
       <c r="E341" s="1"/>
@@ -5490,9 +5491,9 @@
       <c r="A342" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="B342" s="13"/>
-      <c r="C342" s="13"/>
-      <c r="D342" s="13"/>
+      <c r="B342" s="14"/>
+      <c r="C342" s="14"/>
+      <c r="D342" s="14"/>
       <c r="E342" s="1"/>
     </row>
     <row r="343" spans="1:5" ht="15.75" customHeight="1">
@@ -7061,11 +7062,11 @@
       </c>
       <c r="C501" s="3">
         <f t="shared" si="0"/>
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D501" s="1">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E501" s="1">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Fixes #20 and fixes #21
Added Little Swift and Indian Peafowl.Change the image of Kaju Kele. Added word Weras ganga.
</commit_message>
<xml_diff>
--- a/old_vs_new_records.xlsx
+++ b/old_vs_new_records.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Projects\Mora-Bird-Diversity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65CC9AB1-5F91-4715-AEAB-6CB2DD9849D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{669CD885-AA25-4C6F-A263-378384471DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1791,7 +1791,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1832,6 +1832,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF1C232"/>
         <bgColor rgb="FFF1C232"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1895,7 +1901,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1920,6 +1926,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2137,24 +2144,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A488" workbookViewId="0">
-      <selection activeCell="H506" sqref="H506"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="53.44140625" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" customWidth="1"/>
+    <col min="1" max="1" width="53.42578125" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" customWidth="1"/>
     <col min="3" max="3" width="8" customWidth="1"/>
     <col min="4" max="4" width="4" customWidth="1"/>
-    <col min="5" max="5" width="3.88671875" customWidth="1"/>
-    <col min="6" max="6" width="7.6640625" customWidth="1"/>
-    <col min="7" max="7" width="3.88671875" customWidth="1"/>
-    <col min="8" max="8" width="30.88671875" customWidth="1"/>
-    <col min="9" max="26" width="8.6640625" customWidth="1"/>
+    <col min="5" max="5" width="3.85546875" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" customWidth="1"/>
+    <col min="7" max="7" width="3.85546875" customWidth="1"/>
+    <col min="8" max="8" width="30.85546875" customWidth="1"/>
+    <col min="9" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.4">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2167,14 +2174,14 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="14.4">
+    <row r="2" spans="1:8">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="14.4">
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -2186,7 +2193,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="14.4">
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -2198,7 +2205,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="14.4">
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -2207,7 +2214,7 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:8" ht="14.4">
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -2216,7 +2223,7 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:8" ht="14.4">
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -2225,7 +2232,7 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:8" ht="14.4">
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -2234,7 +2241,7 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:8" ht="14.4">
+    <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -2243,7 +2250,7 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:8" ht="14.4">
+    <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -2252,7 +2259,7 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:8" ht="14.4">
+    <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -2261,7 +2268,7 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:8" ht="14.4">
+    <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -2270,7 +2277,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:8" ht="14.4">
+    <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -2279,7 +2286,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:8" ht="14.4">
+    <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -2288,7 +2295,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:8" ht="14.4">
+    <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -2297,7 +2304,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:8" ht="14.4">
+    <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -2306,7 +2313,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" ht="14.4">
+    <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -2315,7 +2322,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" ht="14.4">
+    <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -2324,7 +2331,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" ht="14.4">
+    <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -2333,7 +2340,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" ht="14.4">
+    <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -2624,7 +2631,7 @@
       <c r="C45" s="3">
         <v>1</v>
       </c>
-      <c r="D45" s="17"/>
+      <c r="D45" s="1"/>
       <c r="E45" s="1"/>
     </row>
     <row r="46" spans="1:5" ht="15.75" customHeight="1">
@@ -3410,9 +3417,13 @@
         <v>129</v>
       </c>
       <c r="B128" s="2"/>
-      <c r="C128" s="3"/>
+      <c r="C128" s="3">
+        <v>1</v>
+      </c>
       <c r="D128" s="1"/>
-      <c r="E128" s="1"/>
+      <c r="E128" s="18">
+        <v>1</v>
+      </c>
     </row>
     <row r="129" spans="1:5" ht="15.75" customHeight="1">
       <c r="A129" s="1" t="s">
@@ -4988,10 +4999,10 @@
       <c r="B292" s="2">
         <v>1</v>
       </c>
-      <c r="C292" s="3"/>
-      <c r="D292" s="7">
-        <v>1</v>
-      </c>
+      <c r="C292" s="3">
+        <v>1</v>
+      </c>
+      <c r="D292" s="17"/>
       <c r="E292" s="1"/>
     </row>
     <row r="293" spans="1:5" ht="15.75" customHeight="1">
@@ -7062,15 +7073,15 @@
       </c>
       <c r="C501" s="3">
         <f t="shared" si="0"/>
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D501" s="1">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E501" s="1">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="502" spans="1:5" ht="15.75" customHeight="1">

</xml_diff>